<commit_message>
Daily attendance processing - 2025-09-30 03:24:00
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_surgery_1_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_surgery_1_session_analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="G90" s="2" t="inlineStr">
         <is>
-          <t>dnasr281@gmail.com, admin@admin.com</t>
+          <t>admin@admin.com, dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H90" s="2" t="inlineStr">
@@ -6087,7 +6087,7 @@
       </c>
       <c r="G116" s="2" t="inlineStr">
         <is>
-          <t>dnasr281@gmail.com, admin@admin.com</t>
+          <t>admin@admin.com, dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H116" s="2" t="inlineStr">
@@ -7241,7 +7241,7 @@
       </c>
       <c r="G142" s="2" t="inlineStr">
         <is>
-          <t>dnasr281@gmail.com, admin@admin.com</t>
+          <t>admin@admin.com, dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H142" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Update attendance report: Y4_B2526_General_&_Special_surgery_1_session_analysis.xlsx
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_surgery_1_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_surgery_1_session_analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -581,12 +581,12 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>system, backup@backdoor.com</t>
+          <t>backup@backdoor.com</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>33/53</t>
+          <t>32/53</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
@@ -800,12 +800,12 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>44/53</t>
+          <t>43/53</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -874,7 +874,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -985,7 +985,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>42.8%</t>
+          <t>40.9%</t>
         </is>
       </c>
     </row>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>62.2%</t>
+          <t>61.4%</t>
         </is>
       </c>
     </row>
@@ -1126,12 +1126,12 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>31/53</t>
+          <t>30/53</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
@@ -1173,12 +1173,12 @@
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>36/53</t>
+          <t>35/53</t>
         </is>
       </c>
       <c r="I13" s="2" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="S15" s="4" t="inlineStr">
         <is>
-          <t>60.1%</t>
+          <t>59.4%</t>
         </is>
       </c>
     </row>
@@ -1573,22 +1573,22 @@
         <v>26</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P18" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R18" s="4" t="inlineStr">
         <is>
-          <t>42.3%</t>
+          <t>38.5%</t>
         </is>
       </c>
       <c r="S18" s="4" t="inlineStr">
         <is>
-          <t>64.4%</t>
+          <t>63.0%</t>
         </is>
       </c>
     </row>
@@ -1651,22 +1651,22 @@
         <v>26</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P19" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R19" s="4" t="inlineStr">
         <is>
-          <t>42.3%</t>
+          <t>38.5%</t>
         </is>
       </c>
       <c r="S19" s="4" t="inlineStr">
         <is>
-          <t>67.6%</t>
+          <t>67.3%</t>
         </is>
       </c>
     </row>
@@ -1729,22 +1729,22 @@
         <v>26</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P20" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R20" s="4" t="inlineStr">
         <is>
-          <t>42.3%</t>
+          <t>38.5%</t>
         </is>
       </c>
       <c r="S20" s="4" t="inlineStr">
         <is>
-          <t>71.6%</t>
+          <t>70.4%</t>
         </is>
       </c>
     </row>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>system, backup@backdoor.com</t>
+          <t>backup@backdoor.com</t>
         </is>
       </c>
       <c r="H29" s="2" t="inlineStr">
@@ -2374,7 +2374,7 @@
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H33" s="2" t="inlineStr">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H39" s="2" t="inlineStr">
@@ -2703,7 +2703,7 @@
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H40" s="2" t="inlineStr">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
-          <t>system, backup@backdoor.com</t>
+          <t>backup@backdoor.com</t>
         </is>
       </c>
       <c r="H56" s="2" t="inlineStr">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="G66" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H66" s="2" t="inlineStr">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="G67" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H67" s="2" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="G90" s="2" t="inlineStr">
         <is>
-          <t>admin@admin.com, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com, admin@admin.com</t>
         </is>
       </c>
       <c r="H90" s="2" t="inlineStr">
@@ -5032,7 +5032,7 @@
       </c>
       <c r="H92" s="2" t="inlineStr">
         <is>
-          <t>43/56</t>
+          <t>45/56</t>
         </is>
       </c>
       <c r="I92" s="2" t="inlineStr">
@@ -5042,49 +5042,45 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B93" s="2" t="inlineStr">
+      <c r="A93" s="9" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B93" s="9" t="inlineStr">
         <is>
           <t>B2D</t>
         </is>
       </c>
-      <c r="C93" s="2" t="inlineStr">
-        <is>
-          <t>GENERAL SURGERY</t>
-        </is>
-      </c>
-      <c r="D93" s="2" t="inlineStr">
+      <c r="C93" s="9" t="inlineStr">
+        <is>
+          <t>GENERAL SURGERY</t>
+        </is>
+      </c>
+      <c r="D93" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E93" s="2" t="inlineStr">
+      <c r="E93" s="9" t="inlineStr">
         <is>
           <t>01/10/2025</t>
         </is>
       </c>
-      <c r="F93" s="2" t="inlineStr">
-        <is>
-          <t>10:30:00</t>
-        </is>
-      </c>
-      <c r="G93" s="2" t="inlineStr">
-        <is>
-          <t>dnasr281@gmail.com</t>
-        </is>
-      </c>
-      <c r="H93" s="2" t="inlineStr">
-        <is>
-          <t>46/56</t>
-        </is>
-      </c>
-      <c r="I93" s="2" t="inlineStr">
-        <is>
-          <t>Recorded</t>
+      <c r="F93" s="9" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G93" s="9" t="inlineStr"/>
+      <c r="H93" s="9" t="inlineStr">
+        <is>
+          <t>0/56</t>
+        </is>
+      </c>
+      <c r="I93" s="9" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -6095,7 +6091,7 @@
       </c>
       <c r="G116" s="2" t="inlineStr">
         <is>
-          <t>admin@admin.com, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com, admin@admin.com</t>
         </is>
       </c>
       <c r="H116" s="2" t="inlineStr">
@@ -6194,7 +6190,7 @@
       </c>
       <c r="H118" s="2" t="inlineStr">
         <is>
-          <t>45/55</t>
+          <t>46/55</t>
         </is>
       </c>
       <c r="I118" s="2" t="inlineStr">
@@ -6204,49 +6200,45 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B119" s="2" t="inlineStr">
+      <c r="A119" s="9" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B119" s="9" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C119" s="2" t="inlineStr">
-        <is>
-          <t>GENERAL SURGERY</t>
-        </is>
-      </c>
-      <c r="D119" s="2" t="inlineStr">
+      <c r="C119" s="9" t="inlineStr">
+        <is>
+          <t>GENERAL SURGERY</t>
+        </is>
+      </c>
+      <c r="D119" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E119" s="2" t="inlineStr">
+      <c r="E119" s="9" t="inlineStr">
         <is>
           <t>01/10/2025</t>
         </is>
       </c>
-      <c r="F119" s="2" t="inlineStr">
-        <is>
-          <t>10:30:00</t>
-        </is>
-      </c>
-      <c r="G119" s="2" t="inlineStr">
-        <is>
-          <t>dnasr281@gmail.com</t>
-        </is>
-      </c>
-      <c r="H119" s="2" t="inlineStr">
-        <is>
-          <t>40/55</t>
-        </is>
-      </c>
-      <c r="I119" s="2" t="inlineStr">
-        <is>
-          <t>Recorded</t>
+      <c r="F119" s="9" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G119" s="9" t="inlineStr"/>
+      <c r="H119" s="9" t="inlineStr">
+        <is>
+          <t>0/55</t>
+        </is>
+      </c>
+      <c r="I119" s="9" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -7257,7 +7249,7 @@
       </c>
       <c r="G142" s="2" t="inlineStr">
         <is>
-          <t>admin@admin.com, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com, admin@admin.com</t>
         </is>
       </c>
       <c r="H142" s="2" t="inlineStr">
@@ -7366,49 +7358,45 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="2" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B145" s="2" t="inlineStr">
+      <c r="A145" s="9" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B145" s="9" t="inlineStr">
         <is>
           <t>B2F</t>
         </is>
       </c>
-      <c r="C145" s="2" t="inlineStr">
-        <is>
-          <t>GENERAL SURGERY</t>
-        </is>
-      </c>
-      <c r="D145" s="2" t="inlineStr">
+      <c r="C145" s="9" t="inlineStr">
+        <is>
+          <t>GENERAL SURGERY</t>
+        </is>
+      </c>
+      <c r="D145" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E145" s="2" t="inlineStr">
+      <c r="E145" s="9" t="inlineStr">
         <is>
           <t>01/10/2025</t>
         </is>
       </c>
-      <c r="F145" s="2" t="inlineStr">
-        <is>
-          <t>10:30:00</t>
-        </is>
-      </c>
-      <c r="G145" s="2" t="inlineStr">
-        <is>
-          <t>dnasr281@gmail.com</t>
-        </is>
-      </c>
-      <c r="H145" s="2" t="inlineStr">
-        <is>
-          <t>48/57</t>
-        </is>
-      </c>
-      <c r="I145" s="2" t="inlineStr">
-        <is>
-          <t>Recorded</t>
+      <c r="F145" s="9" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G145" s="9" t="inlineStr"/>
+      <c r="H145" s="9" t="inlineStr">
+        <is>
+          <t>0/57</t>
+        </is>
+      </c>
+      <c r="I145" s="9" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Upload Y4_B2526_General_&_Special_surgery_1_session_analysis.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_surgery_1_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_surgery_1_session_analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -581,12 +581,12 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>system, backup@backdoor.com</t>
+          <t>backup@backdoor.com</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>33/53</t>
+          <t>32/53</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
@@ -800,12 +800,12 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>44/53</t>
+          <t>43/53</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -874,7 +874,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -985,7 +985,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>42.8%</t>
+          <t>40.9%</t>
         </is>
       </c>
     </row>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>62.2%</t>
+          <t>61.4%</t>
         </is>
       </c>
     </row>
@@ -1126,12 +1126,12 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
-          <t>31/53</t>
+          <t>30/53</t>
         </is>
       </c>
       <c r="I12" s="2" t="inlineStr">
@@ -1173,12 +1173,12 @@
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>36/53</t>
+          <t>35/53</t>
         </is>
       </c>
       <c r="I13" s="2" t="inlineStr">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="S15" s="4" t="inlineStr">
         <is>
-          <t>60.1%</t>
+          <t>59.4%</t>
         </is>
       </c>
     </row>
@@ -1573,22 +1573,22 @@
         <v>26</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P18" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R18" s="4" t="inlineStr">
         <is>
-          <t>42.3%</t>
+          <t>38.5%</t>
         </is>
       </c>
       <c r="S18" s="4" t="inlineStr">
         <is>
-          <t>64.4%</t>
+          <t>63.0%</t>
         </is>
       </c>
     </row>
@@ -1651,22 +1651,22 @@
         <v>26</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P19" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R19" s="4" t="inlineStr">
         <is>
-          <t>42.3%</t>
+          <t>38.5%</t>
         </is>
       </c>
       <c r="S19" s="4" t="inlineStr">
         <is>
-          <t>67.6%</t>
+          <t>67.3%</t>
         </is>
       </c>
     </row>
@@ -1729,22 +1729,22 @@
         <v>26</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P20" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R20" s="4" t="inlineStr">
         <is>
-          <t>42.3%</t>
+          <t>38.5%</t>
         </is>
       </c>
       <c r="S20" s="4" t="inlineStr">
         <is>
-          <t>71.6%</t>
+          <t>70.4%</t>
         </is>
       </c>
     </row>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>system, backup@backdoor.com</t>
+          <t>backup@backdoor.com</t>
         </is>
       </c>
       <c r="H29" s="2" t="inlineStr">
@@ -2374,7 +2374,7 @@
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H33" s="2" t="inlineStr">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H39" s="2" t="inlineStr">
@@ -2703,7 +2703,7 @@
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H40" s="2" t="inlineStr">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
-          <t>system, backup@backdoor.com</t>
+          <t>backup@backdoor.com</t>
         </is>
       </c>
       <c r="H56" s="2" t="inlineStr">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="G66" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H66" s="2" t="inlineStr">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="G67" s="2" t="inlineStr">
         <is>
-          <t>System, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com</t>
         </is>
       </c>
       <c r="H67" s="2" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="G90" s="2" t="inlineStr">
         <is>
-          <t>admin@admin.com, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com, admin@admin.com</t>
         </is>
       </c>
       <c r="H90" s="2" t="inlineStr">
@@ -5032,7 +5032,7 @@
       </c>
       <c r="H92" s="2" t="inlineStr">
         <is>
-          <t>43/56</t>
+          <t>45/56</t>
         </is>
       </c>
       <c r="I92" s="2" t="inlineStr">
@@ -5042,49 +5042,45 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B93" s="2" t="inlineStr">
+      <c r="A93" s="9" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B93" s="9" t="inlineStr">
         <is>
           <t>B2D</t>
         </is>
       </c>
-      <c r="C93" s="2" t="inlineStr">
-        <is>
-          <t>GENERAL SURGERY</t>
-        </is>
-      </c>
-      <c r="D93" s="2" t="inlineStr">
+      <c r="C93" s="9" t="inlineStr">
+        <is>
+          <t>GENERAL SURGERY</t>
+        </is>
+      </c>
+      <c r="D93" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E93" s="2" t="inlineStr">
+      <c r="E93" s="9" t="inlineStr">
         <is>
           <t>01/10/2025</t>
         </is>
       </c>
-      <c r="F93" s="2" t="inlineStr">
-        <is>
-          <t>10:30:00</t>
-        </is>
-      </c>
-      <c r="G93" s="2" t="inlineStr">
-        <is>
-          <t>dnasr281@gmail.com</t>
-        </is>
-      </c>
-      <c r="H93" s="2" t="inlineStr">
-        <is>
-          <t>46/56</t>
-        </is>
-      </c>
-      <c r="I93" s="2" t="inlineStr">
-        <is>
-          <t>Recorded</t>
+      <c r="F93" s="9" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G93" s="9" t="inlineStr"/>
+      <c r="H93" s="9" t="inlineStr">
+        <is>
+          <t>0/56</t>
+        </is>
+      </c>
+      <c r="I93" s="9" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -6095,7 +6091,7 @@
       </c>
       <c r="G116" s="2" t="inlineStr">
         <is>
-          <t>admin@admin.com, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com, admin@admin.com</t>
         </is>
       </c>
       <c r="H116" s="2" t="inlineStr">
@@ -6194,7 +6190,7 @@
       </c>
       <c r="H118" s="2" t="inlineStr">
         <is>
-          <t>45/55</t>
+          <t>46/55</t>
         </is>
       </c>
       <c r="I118" s="2" t="inlineStr">
@@ -6204,49 +6200,45 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B119" s="2" t="inlineStr">
+      <c r="A119" s="9" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B119" s="9" t="inlineStr">
         <is>
           <t>B2E</t>
         </is>
       </c>
-      <c r="C119" s="2" t="inlineStr">
-        <is>
-          <t>GENERAL SURGERY</t>
-        </is>
-      </c>
-      <c r="D119" s="2" t="inlineStr">
+      <c r="C119" s="9" t="inlineStr">
+        <is>
+          <t>GENERAL SURGERY</t>
+        </is>
+      </c>
+      <c r="D119" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E119" s="2" t="inlineStr">
+      <c r="E119" s="9" t="inlineStr">
         <is>
           <t>01/10/2025</t>
         </is>
       </c>
-      <c r="F119" s="2" t="inlineStr">
-        <is>
-          <t>10:30:00</t>
-        </is>
-      </c>
-      <c r="G119" s="2" t="inlineStr">
-        <is>
-          <t>dnasr281@gmail.com</t>
-        </is>
-      </c>
-      <c r="H119" s="2" t="inlineStr">
-        <is>
-          <t>40/55</t>
-        </is>
-      </c>
-      <c r="I119" s="2" t="inlineStr">
-        <is>
-          <t>Recorded</t>
+      <c r="F119" s="9" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G119" s="9" t="inlineStr"/>
+      <c r="H119" s="9" t="inlineStr">
+        <is>
+          <t>0/55</t>
+        </is>
+      </c>
+      <c r="I119" s="9" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -7257,7 +7249,7 @@
       </c>
       <c r="G142" s="2" t="inlineStr">
         <is>
-          <t>admin@admin.com, dnasr281@gmail.com</t>
+          <t>dnasr281@gmail.com, admin@admin.com</t>
         </is>
       </c>
       <c r="H142" s="2" t="inlineStr">
@@ -7366,49 +7358,45 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="2" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B145" s="2" t="inlineStr">
+      <c r="A145" s="9" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B145" s="9" t="inlineStr">
         <is>
           <t>B2F</t>
         </is>
       </c>
-      <c r="C145" s="2" t="inlineStr">
-        <is>
-          <t>GENERAL SURGERY</t>
-        </is>
-      </c>
-      <c r="D145" s="2" t="inlineStr">
+      <c r="C145" s="9" t="inlineStr">
+        <is>
+          <t>GENERAL SURGERY</t>
+        </is>
+      </c>
+      <c r="D145" s="9" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E145" s="2" t="inlineStr">
+      <c r="E145" s="9" t="inlineStr">
         <is>
           <t>01/10/2025</t>
         </is>
       </c>
-      <c r="F145" s="2" t="inlineStr">
-        <is>
-          <t>10:30:00</t>
-        </is>
-      </c>
-      <c r="G145" s="2" t="inlineStr">
-        <is>
-          <t>dnasr281@gmail.com</t>
-        </is>
-      </c>
-      <c r="H145" s="2" t="inlineStr">
-        <is>
-          <t>48/57</t>
-        </is>
-      </c>
-      <c r="I145" s="2" t="inlineStr">
-        <is>
-          <t>Recorded</t>
+      <c r="F145" s="9" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G145" s="9" t="inlineStr"/>
+      <c r="H145" s="9" t="inlineStr">
+        <is>
+          <t>0/57</t>
+        </is>
+      </c>
+      <c r="I145" s="9" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>